<commit_message>
Working to incorporate IonTorrent demultiplexing.
</commit_message>
<xml_diff>
--- a/data/lab_setup/Hectors_tag_primer_plates.xlsx
+++ b/data/lab_setup/Hectors_tag_primer_plates.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="308">
   <si>
     <t xml:space="preserve">Tag primers location</t>
   </si>
@@ -84,18 +84,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCTAAGGTAACGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCTAAGGTAACGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -146,18 +146,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTAAGGAGAACGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTAAGGAGAACGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -175,18 +175,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGAAGAGGATTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGAAGAGGATTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -240,18 +240,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTACCAAGATCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTACCAAGATCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -266,18 +266,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCAGAAGGAACGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCAGAAGGAACGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -331,18 +331,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCTGCAAGTTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCTGCAAGTTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -357,18 +357,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTTCGTGATTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTTCGTGATTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -419,18 +419,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTTCCGATAACGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTTCCGATAACGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -445,18 +445,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTGAGCGGAACGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTGAGCGGAACGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -507,18 +507,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCTGACCGAACGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCTGACCGAACGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -533,18 +533,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTCCTCGAATCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTCCTCGAATCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -589,18 +589,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTAGGTGGTTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTAGGTGGTTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -615,18 +615,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTCTAACGGACGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTCTAACGGACGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -671,18 +671,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTTGGAGTGTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTTGGAGTGTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -697,18 +697,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTCTAGAGGTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTCTAGAGGTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -723,18 +723,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTCTGGATGACGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTCTGGATGACGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -749,18 +749,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTCTATTCGTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTCTATTCGTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -775,18 +775,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGAGGCAATTGCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGAGGCAATTGCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -801,18 +801,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTTAGTCGGACGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTTAGTCGGACGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -827,18 +827,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCAGATCCATCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCAGATCCATCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -853,18 +853,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTCGCAATTACGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTCGCAATTACGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -879,18 +879,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTTCGAGACGCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTTCGAGACGCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -905,18 +905,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTGCCACGAACGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTGCCACGAACGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -931,18 +931,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGAACCTCATTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGAACCTCATTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -957,18 +957,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCCTGAGATACGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCCTGAGATACGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -983,18 +983,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTTACAACCTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTTACAACCTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1009,18 +1009,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGAACCATCCGCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGAACCATCCGCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1035,18 +1035,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGATCCGGAATCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGATCCGGAATCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1061,18 +1061,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTCGACCACTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTCGACCACTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1087,18 +1087,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCGAGGTTATCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCGAGGTTATCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1113,18 +1113,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTCCAAGCTGCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTCCAAGCTGCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1139,18 +1139,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTCTTACACACGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTCTTACACACGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1165,18 +1165,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTTCTCATTGAACGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTTCTCATTGAACGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1191,18 +1191,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTCGCATCGTTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTCGCATCGTTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1217,18 +1217,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTAAGCCATTGTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTAAGCCATTGTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1243,18 +1243,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGAAGGAATCGTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGAAGGAATCGTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1269,18 +1269,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCTTGAGAATGTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCTTGAGAATGTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1295,18 +1295,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTGGAGGACGGACGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTGGAGGACGGACGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1321,18 +1321,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTAACAATCGGCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTAACAATCGGCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1347,18 +1347,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCTGACATAATCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCTGACATAATCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1373,18 +1373,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTTCCACTTCGCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTTCCACTTCGCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1399,18 +1399,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGAGCACGAATCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGAGCACGAATCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1425,18 +1425,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCTTGACACCGCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCTTGACACCGCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1451,18 +1451,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTTGGAGGCCAGCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTTGGAGGCCAGCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1477,18 +1477,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTGGAGCTTCCTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTGGAGCTTCCTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1503,18 +1503,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTCAGTCCGAACGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTCAGTCCGAACGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1529,18 +1529,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTAAGGCAACCACGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTAAGGCAACCACGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1555,18 +1555,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTTCTAAGAGACGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTTCTAAGAGACGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1581,18 +1581,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTCCTAACATAACGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTCCTAACATAACGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1607,18 +1607,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCGGACAATGGCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCGGACAATGGCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1633,18 +1633,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTTGAGCCTATTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTTGAGCCTATTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1659,18 +1659,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCCGCATGGAACGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCCGCATGGAACGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1685,18 +1685,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCTGGCAATCCTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCTGGCAATCCTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1711,18 +1711,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCCGGAGAATCGCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCCGGAGAATCGCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1737,18 +1737,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTCCACCTCCTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTCCACCTCCTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1763,18 +1763,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCAGCATTAATTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCAGCATTAATTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1789,18 +1789,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTCTGGCAACGGCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTCTGGCAACGGCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1815,18 +1815,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTCCTAGAACACGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTCCTAGAACACGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1841,18 +1841,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTCCTTGATGTTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTCCTTGATGTTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1867,18 +1867,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTCTAGCTCTTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTCTAGCTCTTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1893,18 +1893,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTCACTCGGATCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTCACTCGGATCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1919,18 +1919,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTTCCTGCTTCACGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTTCCTGCTTCACGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1945,18 +1945,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCCTTAGAGTTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCCTTAGAGTTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1971,18 +1971,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCTGAGTTCCGACGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCTGAGTTCCGACGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -1997,18 +1997,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTCCTGGCACATCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTCCTGGCACATCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2023,18 +2023,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCCGCAATCATCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCCGCAATCATCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2049,18 +2049,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTTCCTACCAGTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTTCCTACCAGTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2075,18 +2075,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTCAAGAAGTTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTCAAGAAGTTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2101,18 +2101,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTTCAATTGGCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTTCAATTGGCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2127,18 +2127,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCCTACTGGTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCCTACTGGTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2153,18 +2153,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTGAGGCTCCGACGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTGAGGCTCCGACGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2179,18 +2179,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCGAAGGCCACACGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCGAAGGCCACACGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2205,18 +2205,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTCTGCCTGTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTCTGCCTGTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2231,18 +2231,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCGATCGGTTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCGATCGGTTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2257,18 +2257,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTCAGGAATACGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTCAGGAATACGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2283,18 +2283,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCGGAAGAACCTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCGGAAGAACCTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2309,18 +2309,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCGAAGCGATTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCGAAGCGATTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2335,18 +2335,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCAGCCAATTCTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCAGCCAATTCTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2361,18 +2361,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCCTGGTTGTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCCTGGTTGTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2387,18 +2387,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTCGAAGGCAGGCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTCGAAGGCAGGCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2413,18 +2413,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCCTGCCATTCGCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCCTGCCATTCGCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2439,18 +2439,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTTGGCATCTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTTGGCATCTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2465,18 +2465,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCTAGGACATTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCTAGGACATTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2491,18 +2491,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCTTCCATAACGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCTTCCATAACGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2517,18 +2517,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCCAGCCTCAACGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCCAGCCTCAACGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2543,18 +2543,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCTTGGTTATTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCTTGGTTATTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2569,18 +2569,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTTGGCTGGACGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTTGGCTGGACGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2595,18 +2595,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCCGAACACTTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCCGAACACTTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2621,18 +2621,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTCCTGAATCTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTCCTGAATCTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2647,18 +2647,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCTAACCACGGCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCTAACCACGGCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2673,18 +2673,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCGGAAGGATGCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCGGAAGGATGCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2699,18 +2699,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCTAGGAACCGCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCTAGGAACCGCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2725,18 +2725,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCTTGTCCAATCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCTTGTCCAATCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2751,18 +2751,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTCCGACAAGCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTCCGACAAGCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2777,18 +2777,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGCGGACAGATCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGCGGACAGATCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2803,18 +2803,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCATCTCATCCCTGCGTGTCTCCGACTCAGTTAAGCGGTCGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>GTGARTCATCGARTCTTTG</t>
+      <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAGTTAAGCGGTCGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GTGARTCATCGARTCTTTG</t>
     </r>
   </si>
   <si>
@@ -2853,18 +2853,18 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCTCTCTATGGGCAGTCGGTGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>TCCTCCGCTTATTGATATGC</t>
+      <t xml:space="preserve">CCTCTCTATGGGCAGTCGGTGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">TCCTCCGCTTATTGATATGC</t>
     </r>
   </si>
   <si>
@@ -2879,19 +2879,31 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t>CCTCTCTATGGGCAGTCGGTGAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t>TCCTCGCCTTATTGATATGC</t>
-    </r>
+      <t xml:space="preserve">CCTCTCTATGGGCAGTCGGTGAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">TCCTCGCCTTATTGATATGC</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Ion-A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCATCTCATCCCTGCGTGTCTCCGACTCAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ion-P1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCTCTCTATGGGCAGTCGGTGAT</t>
   </si>
 </sst>
 </file>
@@ -2901,7 +2913,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -2961,6 +2973,12 @@
       <name val="Courier New"/>
       <family val="3"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -3055,7 +3073,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3095,6 +3113,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3103,15 +3125,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3132,22 +3150,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:Q104"/>
+  <dimension ref="B1:Q106"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G79" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P107" activeCellId="0" sqref="P107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0555555555556"/>
-    <col collapsed="false" hidden="false" max="10" min="2" style="0" width="4.3"/>
-    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="5.77037037037037"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.0555555555556"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="10.8185185185185"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="17.0111111111111"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="84.4333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="11.0555555555556"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3209302325581"/>
+    <col collapsed="false" hidden="false" max="10" min="2" style="0" width="4.30697674418605"/>
+    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="5.90697674418605"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.3209302325581"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="11.2"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="17.4744186046512"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="86.8837209302326"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="11.3209302325581"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3262,57 +3280,57 @@
       <c r="P3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="Q3" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J4" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="13" t="s">
+      <c r="K4" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="13" t="s">
+      <c r="L4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="13" t="s">
+      <c r="M4" s="14" t="s">
         <v>30</v>
       </c>
       <c r="N4" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="O4" s="14" t="s">
+      <c r="O4" s="10" t="s">
         <v>10</v>
       </c>
       <c r="P4" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="Q4" s="0" t="s">
+      <c r="Q4" s="12" t="s">
         <v>32</v>
       </c>
     </row>
@@ -3362,57 +3380,57 @@
       <c r="P5" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="Q5" s="0" t="s">
+      <c r="Q5" s="12" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="J6" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="K6" s="13" t="s">
+      <c r="K6" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="L6" s="13" t="s">
+      <c r="L6" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="M6" s="13" t="s">
+      <c r="M6" s="14" t="s">
         <v>47</v>
       </c>
       <c r="N6" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="O6" s="14" t="s">
+      <c r="O6" s="10" t="s">
         <v>48</v>
       </c>
       <c r="P6" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="Q6" s="0" t="s">
+      <c r="Q6" s="12" t="s">
         <v>50</v>
       </c>
     </row>
@@ -3462,57 +3480,57 @@
       <c r="P7" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="Q7" s="0" t="s">
+      <c r="Q7" s="12" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="J8" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="K8" s="13" t="s">
+      <c r="K8" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="L8" s="13" t="s">
+      <c r="L8" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="M8" s="13" t="s">
+      <c r="M8" s="14" t="s">
         <v>64</v>
       </c>
       <c r="N8" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="O8" s="14" t="s">
+      <c r="O8" s="10" t="s">
         <v>65</v>
       </c>
       <c r="P8" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="Q8" s="0" t="s">
+      <c r="Q8" s="12" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3562,57 +3580,57 @@
       <c r="P9" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="Q9" s="0" t="s">
+      <c r="Q9" s="12" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="H10" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="J10" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="K10" s="13" t="s">
+      <c r="K10" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="L10" s="13" t="s">
+      <c r="L10" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="M10" s="13" t="s">
+      <c r="M10" s="14" t="s">
         <v>80</v>
       </c>
       <c r="N10" s="9" t="n">
         <v>8</v>
       </c>
-      <c r="O10" s="14" t="s">
+      <c r="O10" s="10" t="s">
         <v>81</v>
       </c>
       <c r="P10" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="Q10" s="0" t="s">
+      <c r="Q10" s="12" t="s">
         <v>83</v>
       </c>
     </row>
@@ -3662,57 +3680,57 @@
       <c r="P11" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="Q11" s="0" t="s">
+      <c r="Q11" s="12" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="H12" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="I12" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="J12" s="13" t="s">
+      <c r="J12" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="K12" s="13" t="s">
+      <c r="K12" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="L12" s="13" t="s">
+      <c r="L12" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="M12" s="13" t="s">
+      <c r="M12" s="14" t="s">
         <v>97</v>
       </c>
       <c r="N12" s="9" t="n">
         <v>10</v>
       </c>
-      <c r="O12" s="14" t="s">
+      <c r="O12" s="10" t="s">
         <v>30</v>
       </c>
       <c r="P12" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="Q12" s="0" t="s">
+      <c r="Q12" s="12" t="s">
         <v>99</v>
       </c>
     </row>
@@ -3762,57 +3780,57 @@
       <c r="P13" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="Q13" s="0" t="s">
+      <c r="Q13" s="12" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="H14" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="I14" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="J14" s="13" t="s">
+      <c r="J14" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="K14" s="13" t="s">
+      <c r="K14" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="L14" s="13" t="s">
+      <c r="L14" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="M14" s="13" t="s">
+      <c r="M14" s="14" t="s">
         <v>111</v>
       </c>
       <c r="N14" s="9" t="n">
         <v>12</v>
       </c>
-      <c r="O14" s="14" t="s">
+      <c r="O14" s="10" t="s">
         <v>74</v>
       </c>
       <c r="P14" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="Q14" s="0" t="s">
+      <c r="Q14" s="12" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3862,57 +3880,57 @@
       <c r="P15" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="Q15" s="0" t="s">
+      <c r="Q15" s="12" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="G16" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="H16" s="13" t="s">
+      <c r="H16" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="I16" s="13" t="s">
+      <c r="I16" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="J16" s="13" t="s">
+      <c r="J16" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="K16" s="13" t="s">
+      <c r="K16" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="L16" s="13" t="s">
+      <c r="L16" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="M16" s="13" t="s">
+      <c r="M16" s="14" t="s">
         <v>125</v>
       </c>
       <c r="N16" s="9" t="n">
         <v>14</v>
       </c>
-      <c r="O16" s="14" t="s">
+      <c r="O16" s="10" t="s">
         <v>125</v>
       </c>
       <c r="P16" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="Q16" s="0" t="s">
+      <c r="Q16" s="12" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3962,7 +3980,7 @@
       <c r="P17" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="Q17" s="0" t="s">
+      <c r="Q17" s="12" t="s">
         <v>129</v>
       </c>
     </row>
@@ -3976,7 +3994,7 @@
       <c r="P18" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="Q18" s="0" t="s">
+      <c r="Q18" s="12" t="s">
         <v>131</v>
       </c>
     </row>
@@ -3990,7 +4008,7 @@
       <c r="P19" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="Q19" s="0" t="s">
+      <c r="Q19" s="12" t="s">
         <v>133</v>
       </c>
     </row>
@@ -4004,7 +4022,7 @@
       <c r="P20" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="Q20" s="0" t="s">
+      <c r="Q20" s="12" t="s">
         <v>135</v>
       </c>
     </row>
@@ -4018,7 +4036,7 @@
       <c r="P21" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="Q21" s="0" t="s">
+      <c r="Q21" s="12" t="s">
         <v>137</v>
       </c>
     </row>
@@ -4032,7 +4050,7 @@
       <c r="P22" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="Q22" s="0" t="s">
+      <c r="Q22" s="12" t="s">
         <v>139</v>
       </c>
     </row>
@@ -4046,7 +4064,7 @@
       <c r="P23" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="Q23" s="0" t="s">
+      <c r="Q23" s="12" t="s">
         <v>141</v>
       </c>
     </row>
@@ -4060,7 +4078,7 @@
       <c r="P24" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="Q24" s="0" t="s">
+      <c r="Q24" s="12" t="s">
         <v>143</v>
       </c>
     </row>
@@ -4074,7 +4092,7 @@
       <c r="P25" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="Q25" s="0" t="s">
+      <c r="Q25" s="12" t="s">
         <v>145</v>
       </c>
     </row>
@@ -4088,7 +4106,7 @@
       <c r="P26" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="Q26" s="0" t="s">
+      <c r="Q26" s="12" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4102,7 +4120,7 @@
       <c r="P27" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="Q27" s="0" t="s">
+      <c r="Q27" s="12" t="s">
         <v>149</v>
       </c>
     </row>
@@ -4116,7 +4134,7 @@
       <c r="P28" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="Q28" s="0" t="s">
+      <c r="Q28" s="12" t="s">
         <v>151</v>
       </c>
     </row>
@@ -4130,7 +4148,7 @@
       <c r="P29" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="Q29" s="0" t="s">
+      <c r="Q29" s="12" t="s">
         <v>153</v>
       </c>
     </row>
@@ -4144,7 +4162,7 @@
       <c r="P30" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="Q30" s="0" t="s">
+      <c r="Q30" s="12" t="s">
         <v>155</v>
       </c>
     </row>
@@ -4158,7 +4176,7 @@
       <c r="P31" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="Q31" s="0" t="s">
+      <c r="Q31" s="12" t="s">
         <v>157</v>
       </c>
     </row>
@@ -4172,7 +4190,7 @@
       <c r="P32" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="Q32" s="0" t="s">
+      <c r="Q32" s="12" t="s">
         <v>159</v>
       </c>
     </row>
@@ -4186,7 +4204,7 @@
       <c r="P33" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="Q33" s="0" t="s">
+      <c r="Q33" s="12" t="s">
         <v>161</v>
       </c>
     </row>
@@ -4200,7 +4218,7 @@
       <c r="P34" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="Q34" s="0" t="s">
+      <c r="Q34" s="12" t="s">
         <v>163</v>
       </c>
     </row>
@@ -4214,7 +4232,7 @@
       <c r="P35" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="Q35" s="0" t="s">
+      <c r="Q35" s="12" t="s">
         <v>165</v>
       </c>
     </row>
@@ -4228,7 +4246,7 @@
       <c r="P36" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="Q36" s="0" t="s">
+      <c r="Q36" s="12" t="s">
         <v>167</v>
       </c>
     </row>
@@ -4242,7 +4260,7 @@
       <c r="P37" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="Q37" s="0" t="s">
+      <c r="Q37" s="12" t="s">
         <v>169</v>
       </c>
     </row>
@@ -4256,7 +4274,7 @@
       <c r="P38" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="Q38" s="0" t="s">
+      <c r="Q38" s="12" t="s">
         <v>171</v>
       </c>
     </row>
@@ -4270,7 +4288,7 @@
       <c r="P39" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="Q39" s="0" t="s">
+      <c r="Q39" s="12" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4284,7 +4302,7 @@
       <c r="P40" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="Q40" s="0" t="s">
+      <c r="Q40" s="12" t="s">
         <v>175</v>
       </c>
     </row>
@@ -4298,7 +4316,7 @@
       <c r="P41" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="Q41" s="0" t="s">
+      <c r="Q41" s="12" t="s">
         <v>177</v>
       </c>
     </row>
@@ -4312,7 +4330,7 @@
       <c r="P42" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="Q42" s="0" t="s">
+      <c r="Q42" s="12" t="s">
         <v>179</v>
       </c>
     </row>
@@ -4326,7 +4344,7 @@
       <c r="P43" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="Q43" s="0" t="s">
+      <c r="Q43" s="12" t="s">
         <v>181</v>
       </c>
     </row>
@@ -4340,7 +4358,7 @@
       <c r="P44" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="Q44" s="0" t="s">
+      <c r="Q44" s="12" t="s">
         <v>183</v>
       </c>
     </row>
@@ -4354,7 +4372,7 @@
       <c r="P45" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="Q45" s="0" t="s">
+      <c r="Q45" s="12" t="s">
         <v>185</v>
       </c>
     </row>
@@ -4368,7 +4386,7 @@
       <c r="P46" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="Q46" s="0" t="s">
+      <c r="Q46" s="12" t="s">
         <v>187</v>
       </c>
     </row>
@@ -4382,7 +4400,7 @@
       <c r="P47" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="Q47" s="0" t="s">
+      <c r="Q47" s="12" t="s">
         <v>189</v>
       </c>
     </row>
@@ -4396,7 +4414,7 @@
       <c r="P48" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="Q48" s="0" t="s">
+      <c r="Q48" s="12" t="s">
         <v>191</v>
       </c>
     </row>
@@ -4410,7 +4428,7 @@
       <c r="P49" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="Q49" s="0" t="s">
+      <c r="Q49" s="12" t="s">
         <v>193</v>
       </c>
     </row>
@@ -4424,7 +4442,7 @@
       <c r="P50" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="Q50" s="0" t="s">
+      <c r="Q50" s="12" t="s">
         <v>195</v>
       </c>
     </row>
@@ -4438,7 +4456,7 @@
       <c r="P51" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="Q51" s="0" t="s">
+      <c r="Q51" s="12" t="s">
         <v>197</v>
       </c>
     </row>
@@ -4452,7 +4470,7 @@
       <c r="P52" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="Q52" s="0" t="s">
+      <c r="Q52" s="12" t="s">
         <v>199</v>
       </c>
     </row>
@@ -4466,7 +4484,7 @@
       <c r="P53" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="Q53" s="0" t="s">
+      <c r="Q53" s="12" t="s">
         <v>201</v>
       </c>
     </row>
@@ -4480,7 +4498,7 @@
       <c r="P54" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="Q54" s="0" t="s">
+      <c r="Q54" s="12" t="s">
         <v>203</v>
       </c>
     </row>
@@ -4494,7 +4512,7 @@
       <c r="P55" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="Q55" s="0" t="s">
+      <c r="Q55" s="12" t="s">
         <v>205</v>
       </c>
     </row>
@@ -4508,7 +4526,7 @@
       <c r="P56" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="Q56" s="0" t="s">
+      <c r="Q56" s="12" t="s">
         <v>207</v>
       </c>
     </row>
@@ -4522,7 +4540,7 @@
       <c r="P57" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="Q57" s="0" t="s">
+      <c r="Q57" s="12" t="s">
         <v>209</v>
       </c>
     </row>
@@ -4536,7 +4554,7 @@
       <c r="P58" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="Q58" s="0" t="s">
+      <c r="Q58" s="12" t="s">
         <v>211</v>
       </c>
     </row>
@@ -4550,7 +4568,7 @@
       <c r="P59" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="Q59" s="0" t="s">
+      <c r="Q59" s="12" t="s">
         <v>213</v>
       </c>
     </row>
@@ -4564,7 +4582,7 @@
       <c r="P60" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="Q60" s="0" t="s">
+      <c r="Q60" s="12" t="s">
         <v>215</v>
       </c>
     </row>
@@ -4578,7 +4596,7 @@
       <c r="P61" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="Q61" s="0" t="s">
+      <c r="Q61" s="12" t="s">
         <v>217</v>
       </c>
     </row>
@@ -4592,7 +4610,7 @@
       <c r="P62" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="Q62" s="0" t="s">
+      <c r="Q62" s="12" t="s">
         <v>219</v>
       </c>
     </row>
@@ -4606,7 +4624,7 @@
       <c r="P63" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="Q63" s="0" t="s">
+      <c r="Q63" s="12" t="s">
         <v>221</v>
       </c>
     </row>
@@ -4620,7 +4638,7 @@
       <c r="P64" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="Q64" s="0" t="s">
+      <c r="Q64" s="12" t="s">
         <v>223</v>
       </c>
     </row>
@@ -4634,7 +4652,7 @@
       <c r="P65" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="Q65" s="0" t="s">
+      <c r="Q65" s="12" t="s">
         <v>225</v>
       </c>
     </row>
@@ -4648,7 +4666,7 @@
       <c r="P66" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="Q66" s="0" t="s">
+      <c r="Q66" s="12" t="s">
         <v>227</v>
       </c>
     </row>
@@ -4662,7 +4680,7 @@
       <c r="P67" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="Q67" s="0" t="s">
+      <c r="Q67" s="12" t="s">
         <v>229</v>
       </c>
     </row>
@@ -4676,7 +4694,7 @@
       <c r="P68" s="11" t="s">
         <v>230</v>
       </c>
-      <c r="Q68" s="0" t="s">
+      <c r="Q68" s="12" t="s">
         <v>231</v>
       </c>
     </row>
@@ -4690,7 +4708,7 @@
       <c r="P69" s="11" t="s">
         <v>232</v>
       </c>
-      <c r="Q69" s="0" t="s">
+      <c r="Q69" s="12" t="s">
         <v>233</v>
       </c>
     </row>
@@ -4704,7 +4722,7 @@
       <c r="P70" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="Q70" s="0" t="s">
+      <c r="Q70" s="12" t="s">
         <v>235</v>
       </c>
     </row>
@@ -4718,7 +4736,7 @@
       <c r="P71" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="Q71" s="0" t="s">
+      <c r="Q71" s="12" t="s">
         <v>237</v>
       </c>
     </row>
@@ -4732,7 +4750,7 @@
       <c r="P72" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="Q72" s="0" t="s">
+      <c r="Q72" s="12" t="s">
         <v>239</v>
       </c>
     </row>
@@ -4746,7 +4764,7 @@
       <c r="P73" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="Q73" s="0" t="s">
+      <c r="Q73" s="12" t="s">
         <v>241</v>
       </c>
     </row>
@@ -4760,7 +4778,7 @@
       <c r="P74" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="Q74" s="0" t="s">
+      <c r="Q74" s="12" t="s">
         <v>243</v>
       </c>
     </row>
@@ -4774,7 +4792,7 @@
       <c r="P75" s="11" t="s">
         <v>244</v>
       </c>
-      <c r="Q75" s="0" t="s">
+      <c r="Q75" s="12" t="s">
         <v>245</v>
       </c>
     </row>
@@ -4788,7 +4806,7 @@
       <c r="P76" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="Q76" s="0" t="s">
+      <c r="Q76" s="12" t="s">
         <v>247</v>
       </c>
     </row>
@@ -4802,7 +4820,7 @@
       <c r="P77" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="Q77" s="0" t="s">
+      <c r="Q77" s="12" t="s">
         <v>249</v>
       </c>
     </row>
@@ -4816,7 +4834,7 @@
       <c r="P78" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="Q78" s="0" t="s">
+      <c r="Q78" s="12" t="s">
         <v>251</v>
       </c>
     </row>
@@ -4830,7 +4848,7 @@
       <c r="P79" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="Q79" s="0" t="s">
+      <c r="Q79" s="12" t="s">
         <v>253</v>
       </c>
     </row>
@@ -4844,7 +4862,7 @@
       <c r="P80" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="Q80" s="0" t="s">
+      <c r="Q80" s="12" t="s">
         <v>255</v>
       </c>
     </row>
@@ -4858,7 +4876,7 @@
       <c r="P81" s="11" t="s">
         <v>256</v>
       </c>
-      <c r="Q81" s="0" t="s">
+      <c r="Q81" s="12" t="s">
         <v>257</v>
       </c>
     </row>
@@ -4872,7 +4890,7 @@
       <c r="P82" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="Q82" s="0" t="s">
+      <c r="Q82" s="12" t="s">
         <v>259</v>
       </c>
     </row>
@@ -4886,7 +4904,7 @@
       <c r="P83" s="11" t="s">
         <v>260</v>
       </c>
-      <c r="Q83" s="0" t="s">
+      <c r="Q83" s="12" t="s">
         <v>261</v>
       </c>
     </row>
@@ -4900,7 +4918,7 @@
       <c r="P84" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="Q84" s="0" t="s">
+      <c r="Q84" s="12" t="s">
         <v>263</v>
       </c>
     </row>
@@ -4914,7 +4932,7 @@
       <c r="P85" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="Q85" s="0" t="s">
+      <c r="Q85" s="12" t="s">
         <v>265</v>
       </c>
     </row>
@@ -4928,7 +4946,7 @@
       <c r="P86" s="11" t="s">
         <v>266</v>
       </c>
-      <c r="Q86" s="0" t="s">
+      <c r="Q86" s="12" t="s">
         <v>267</v>
       </c>
     </row>
@@ -4942,7 +4960,7 @@
       <c r="P87" s="11" t="s">
         <v>268</v>
       </c>
-      <c r="Q87" s="0" t="s">
+      <c r="Q87" s="12" t="s">
         <v>269</v>
       </c>
     </row>
@@ -4956,7 +4974,7 @@
       <c r="P88" s="11" t="s">
         <v>270</v>
       </c>
-      <c r="Q88" s="0" t="s">
+      <c r="Q88" s="12" t="s">
         <v>271</v>
       </c>
     </row>
@@ -4970,7 +4988,7 @@
       <c r="P89" s="11" t="s">
         <v>272</v>
       </c>
-      <c r="Q89" s="0" t="s">
+      <c r="Q89" s="12" t="s">
         <v>273</v>
       </c>
     </row>
@@ -4984,7 +5002,7 @@
       <c r="P90" s="11" t="s">
         <v>274</v>
       </c>
-      <c r="Q90" s="0" t="s">
+      <c r="Q90" s="12" t="s">
         <v>275</v>
       </c>
     </row>
@@ -4998,7 +5016,7 @@
       <c r="P91" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="Q91" s="0" t="s">
+      <c r="Q91" s="12" t="s">
         <v>277</v>
       </c>
     </row>
@@ -5012,7 +5030,7 @@
       <c r="P92" s="11" t="s">
         <v>278</v>
       </c>
-      <c r="Q92" s="0" t="s">
+      <c r="Q92" s="12" t="s">
         <v>279</v>
       </c>
     </row>
@@ -5026,7 +5044,7 @@
       <c r="P93" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="Q93" s="0" t="s">
+      <c r="Q93" s="12" t="s">
         <v>281</v>
       </c>
     </row>
@@ -5040,7 +5058,7 @@
       <c r="P94" s="11" t="s">
         <v>282</v>
       </c>
-      <c r="Q94" s="0" t="s">
+      <c r="Q94" s="12" t="s">
         <v>283</v>
       </c>
     </row>
@@ -5054,7 +5072,7 @@
       <c r="P95" s="11" t="s">
         <v>284</v>
       </c>
-      <c r="Q95" s="0" t="s">
+      <c r="Q95" s="12" t="s">
         <v>285</v>
       </c>
     </row>
@@ -5068,7 +5086,7 @@
       <c r="P96" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="Q96" s="0" t="s">
+      <c r="Q96" s="12" t="s">
         <v>287</v>
       </c>
     </row>
@@ -5082,11 +5100,11 @@
       <c r="P97" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="Q97" s="0" t="s">
+      <c r="Q97" s="12" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N98" s="9" t="n">
         <v>96</v>
       </c>
@@ -5096,7 +5114,7 @@
       <c r="P98" s="11" t="s">
         <v>290</v>
       </c>
-      <c r="Q98" s="0" t="s">
+      <c r="Q98" s="12" t="s">
         <v>291</v>
       </c>
     </row>
@@ -5136,20 +5154,36 @@
         <v>299</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="P103" s="16" t="s">
+    <row r="103" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P103" s="12" t="s">
         <v>300</v>
       </c>
-      <c r="Q103" s="0" t="s">
+      <c r="Q103" s="12" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="P104" s="16" t="s">
+      <c r="P104" s="12" t="s">
         <v>302</v>
       </c>
-      <c r="Q104" s="0" t="s">
+      <c r="Q104" s="12" t="s">
         <v>303</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P105" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q105" s="16" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P106" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="Q106" s="16" t="s">
+        <v>307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>